<commit_message>
See code in between ############
</commit_message>
<xml_diff>
--- a/Hot_Test_15/Feeding Rate 22 nd June 2023.xlsx
+++ b/Hot_Test_15/Feeding Rate 22 nd June 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/kevin_kung_ubc_ca/Documents/LabJack DataLogging/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zihaowang/PycharmProjects/Time-Series-Analysis/Takachar-Time-Series-Analysis/Hot_Test_15/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="726" documentId="11_935C230D6DB2E9BE6FD1B20575ADDC78C04E0811" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95047619-8106-4F5A-A48F-19CD8230E535}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA2A358-9598-1C45-9BC1-F6B6AD8E1E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5650" yWindow="1300" windowWidth="16460" windowHeight="8730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mass Flow" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
     <numFmt numFmtId="165" formatCode="0.0;0.0;;@"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,7 +391,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2251,63 +2251,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="5"/>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="5"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
     <col min="3" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="7" width="8.7109375" style="3"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="7" width="8.6640625" style="3"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="I8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J8" s="8">
-        <f ca="1">J10/F10</f>
+        <f>J10/F10</f>
         <v>0.26200355810665044</v>
       </c>
       <c r="K8" s="9">
-        <f ca="1">J8/0.764555</f>
+        <f>J8/0.764555</f>
         <v>0.34268765243396543</v>
       </c>
       <c r="L8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -2321,18 +2321,18 @@
         <v>9</v>
       </c>
       <c r="J9" s="9">
-        <f ca="1">J8*((J11/J10)+(F12/F10))</f>
+        <f>J8*((J11/J10)+(F12/F10))</f>
         <v>6.7044107738186151E-3</v>
       </c>
       <c r="K9" s="9">
-        <f ca="1">J9/0.764555</f>
+        <f>J9/0.764555</f>
         <v>8.7690365949063386E-3</v>
       </c>
       <c r="L9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -2356,18 +2356,17 @@
         <v>15</v>
       </c>
       <c r="J10" s="4">
-        <f t="array" aca="1" ref="J10:K14" ca="1">LINEST($E$15:INDEX($E16:$E201,COUNTIF($E$16:$E$201,"&lt;&gt;0")),$A$15:INDEX($A16:$A201,COUNTIF($A$16:$A$201,"&lt;&gt;0")),1,1)</f>
+        <f t="array" ref="J10:K14">LINEST($E$15:INDEX($E16:$E201,COUNTIF($E$16:$E$201,"&lt;&gt;0")),$A$15:INDEX($A16:$A201,COUNTIF($A$16:$A$201,"&lt;&gt;0")),1,1)</f>
         <v>58.085128008059556</v>
       </c>
       <c r="K10" s="3">
-        <f ca="1"/>
         <v>-641.57518658537811</v>
       </c>
       <c r="L10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11">
         <f>C10/1000</f>
         <v>3.85E-2</v>
@@ -2389,18 +2388,16 @@
         <v>19</v>
       </c>
       <c r="J11" s="3">
-        <f ca="1"/>
         <v>0.85966653329798481</v>
       </c>
       <c r="K11" s="3">
-        <f ca="1"/>
         <v>11.715500374663366</v>
       </c>
       <c r="L11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>21</v>
       </c>
@@ -2415,34 +2412,30 @@
         <v>22</v>
       </c>
       <c r="J12" s="3">
-        <f ca="1"/>
         <v>0.99282344360457353</v>
       </c>
       <c r="K12" s="3">
-        <f ca="1"/>
         <v>7.5148368148904297</v>
       </c>
       <c r="L12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I13" t="s">
         <v>24</v>
       </c>
       <c r="J13" s="3">
-        <f ca="1"/>
         <v>4565.3056749934449</v>
       </c>
       <c r="K13" s="3">
-        <f ca="1"/>
         <v>33</v>
       </c>
       <c r="L13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
@@ -2465,18 +2458,16 @@
         <v>32</v>
       </c>
       <c r="J14" s="3">
-        <f ca="1"/>
         <v>257815.46811230379</v>
       </c>
       <c r="K14" s="3">
-        <f ca="1"/>
         <v>1863.6014876962738</v>
       </c>
       <c r="L14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <f>B15*24</f>
         <v>11.25</v>
@@ -2500,7 +2491,7 @@
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <f t="shared" ref="A16:A79" si="2">B16*24</f>
         <v>11.35</v>
@@ -2525,7 +2516,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <f t="shared" si="2"/>
         <v>11.4</v>
@@ -2550,7 +2541,7 @@
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <f t="shared" si="2"/>
         <v>11.7</v>
@@ -2575,7 +2566,7 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <f t="shared" si="2"/>
         <v>11.75</v>
@@ -2600,7 +2591,7 @@
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <f t="shared" si="2"/>
         <v>11.833333333333334</v>
@@ -2625,7 +2616,7 @@
       </c>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <f t="shared" si="2"/>
         <v>11.916666666666666</v>
@@ -2650,7 +2641,7 @@
       </c>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <f t="shared" si="2"/>
         <v>12.033333333333333</v>
@@ -2675,7 +2666,7 @@
       </c>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <f t="shared" si="2"/>
         <v>12.166666666666666</v>
@@ -2700,7 +2691,7 @@
       </c>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <f t="shared" si="2"/>
         <v>12.283333333333331</v>
@@ -2725,7 +2716,7 @@
       </c>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <f t="shared" si="2"/>
         <v>12.416666666666664</v>
@@ -2750,7 +2741,7 @@
       </c>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <f t="shared" si="2"/>
         <v>12.516666666666667</v>
@@ -2775,7 +2766,7 @@
       </c>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <f t="shared" si="2"/>
         <v>12.666666666666668</v>
@@ -2800,7 +2791,7 @@
       </c>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <f t="shared" si="2"/>
         <v>12.75</v>
@@ -2825,7 +2816,7 @@
       </c>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <f t="shared" si="2"/>
         <v>12.85</v>
@@ -2850,7 +2841,7 @@
       </c>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <f t="shared" si="2"/>
         <v>13.316666666666666</v>
@@ -2875,7 +2866,7 @@
       </c>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <f t="shared" si="2"/>
         <v>13.416666666666668</v>
@@ -2900,7 +2891,7 @@
       </c>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <f t="shared" si="2"/>
         <v>13.5</v>
@@ -2925,7 +2916,7 @@
       </c>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <f t="shared" si="2"/>
         <v>13.866666666666667</v>
@@ -2950,7 +2941,7 @@
       </c>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <f t="shared" si="2"/>
         <v>13.966666666666669</v>
@@ -2975,7 +2966,7 @@
       </c>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <f t="shared" si="2"/>
         <v>14.066666666666666</v>
@@ -3000,7 +2991,7 @@
       </c>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <f t="shared" si="2"/>
         <v>14.133333333333333</v>
@@ -3025,7 +3016,7 @@
       </c>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <f t="shared" si="2"/>
         <v>14.366666666666667</v>
@@ -3050,7 +3041,7 @@
       </c>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <f t="shared" si="2"/>
         <v>14.399999999999999</v>
@@ -3075,7 +3066,7 @@
       </c>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <f t="shared" si="2"/>
         <v>14.45</v>
@@ -3100,7 +3091,7 @@
       </c>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <f t="shared" si="2"/>
         <v>14.583333333333336</v>
@@ -3125,7 +3116,7 @@
       </c>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <f t="shared" si="2"/>
         <v>14.850000000000001</v>
@@ -3150,7 +3141,7 @@
       </c>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <f t="shared" si="2"/>
         <v>14.933333333333334</v>
@@ -3175,7 +3166,7 @@
       </c>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -3200,7 +3191,7 @@
       </c>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <f t="shared" si="2"/>
         <v>15.166666666666666</v>
@@ -3225,7 +3216,7 @@
       </c>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <f t="shared" si="2"/>
         <v>15.583333333333334</v>
@@ -3250,7 +3241,7 @@
       </c>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <f t="shared" si="2"/>
         <v>15.733333333333334</v>
@@ -3275,7 +3266,7 @@
       </c>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <f t="shared" si="2"/>
         <v>15.816666666666666</v>
@@ -3300,7 +3291,7 @@
       </c>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <f t="shared" si="2"/>
         <v>15.899999999999999</v>
@@ -3325,7 +3316,7 @@
       </c>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <f t="shared" si="2"/>
         <v>16.233333333333334</v>
@@ -3351,7 +3342,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3372,7 +3363,7 @@
       </c>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3393,7 +3384,7 @@
       </c>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3414,7 +3405,7 @@
       </c>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3435,7 +3426,7 @@
       </c>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3456,7 +3447,7 @@
       </c>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3477,7 +3468,7 @@
       </c>
       <c r="G55" s="5"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3498,7 +3489,7 @@
       </c>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3519,7 +3510,7 @@
       </c>
       <c r="G57" s="5"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3540,7 +3531,7 @@
       </c>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3561,7 +3552,7 @@
       </c>
       <c r="G59" s="5"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3582,7 +3573,7 @@
       </c>
       <c r="G60" s="5"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3603,7 +3594,7 @@
       </c>
       <c r="G61" s="5"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3624,7 +3615,7 @@
       </c>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3645,7 +3636,7 @@
       </c>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3666,7 +3657,7 @@
       </c>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3687,7 +3678,7 @@
       </c>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3708,7 +3699,7 @@
       </c>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3729,7 +3720,7 @@
       </c>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3750,7 +3741,7 @@
       </c>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3771,7 +3762,7 @@
       </c>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3792,7 +3783,7 @@
       </c>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3813,7 +3804,7 @@
       </c>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3834,7 +3825,7 @@
       </c>
       <c r="G72" s="5"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3855,7 +3846,7 @@
       </c>
       <c r="G73" s="5"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3876,7 +3867,7 @@
       </c>
       <c r="G74" s="5"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3897,7 +3888,7 @@
       </c>
       <c r="G75" s="5"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3918,7 +3909,7 @@
       </c>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3939,7 +3930,7 @@
       </c>
       <c r="G77" s="5"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3960,7 +3951,7 @@
       </c>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3981,7 +3972,7 @@
       </c>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
         <f t="shared" ref="A80:A143" si="5">B80*24</f>
         <v>0</v>
@@ -4002,7 +3993,7 @@
       </c>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4023,7 +4014,7 @@
       </c>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4044,7 +4035,7 @@
       </c>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4065,7 +4056,7 @@
       </c>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4086,7 +4077,7 @@
       </c>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4107,7 +4098,7 @@
       </c>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4128,7 +4119,7 @@
       </c>
       <c r="G86" s="5"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4149,7 +4140,7 @@
       </c>
       <c r="G87" s="5"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4170,7 +4161,7 @@
       </c>
       <c r="G88" s="5"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4191,7 +4182,7 @@
       </c>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4212,7 +4203,7 @@
       </c>
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4233,7 +4224,7 @@
       </c>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4254,7 +4245,7 @@
       </c>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4275,7 +4266,7 @@
       </c>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4296,7 +4287,7 @@
       </c>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4317,7 +4308,7 @@
       </c>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4338,7 +4329,7 @@
       </c>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4359,7 +4350,7 @@
       </c>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4380,7 +4371,7 @@
       </c>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4401,7 +4392,7 @@
       </c>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4422,7 +4413,7 @@
       </c>
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4443,7 +4434,7 @@
       </c>
       <c r="G101" s="5"/>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4464,7 +4455,7 @@
       </c>
       <c r="G102" s="5"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4485,7 +4476,7 @@
       </c>
       <c r="G103" s="5"/>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4506,7 +4497,7 @@
       </c>
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4527,7 +4518,7 @@
       </c>
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4548,7 +4539,7 @@
       </c>
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4569,7 +4560,7 @@
       </c>
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4590,7 +4581,7 @@
       </c>
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4611,7 +4602,7 @@
       </c>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4632,7 +4623,7 @@
       </c>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4653,7 +4644,7 @@
       </c>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4674,7 +4665,7 @@
       </c>
       <c r="G112" s="5"/>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4695,7 +4686,7 @@
       </c>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4716,7 +4707,7 @@
       </c>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4737,7 +4728,7 @@
       </c>
       <c r="G115" s="5"/>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4758,7 +4749,7 @@
       </c>
       <c r="G116" s="5"/>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4779,7 +4770,7 @@
       </c>
       <c r="G117" s="5"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4800,7 +4791,7 @@
       </c>
       <c r="G118" s="5"/>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4821,7 +4812,7 @@
       </c>
       <c r="G119" s="5"/>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4842,7 +4833,7 @@
       </c>
       <c r="G120" s="5"/>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4863,7 +4854,7 @@
       </c>
       <c r="G121" s="5"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4884,7 +4875,7 @@
       </c>
       <c r="G122" s="5"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4905,7 +4896,7 @@
       </c>
       <c r="G123" s="5"/>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4926,7 +4917,7 @@
       </c>
       <c r="G124" s="5"/>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4947,7 +4938,7 @@
       </c>
       <c r="G125" s="5"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4968,7 +4959,7 @@
       </c>
       <c r="G126" s="5"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4989,7 +4980,7 @@
       </c>
       <c r="G127" s="5"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5010,7 +5001,7 @@
       </c>
       <c r="G128" s="5"/>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5031,7 +5022,7 @@
       </c>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5052,7 +5043,7 @@
       </c>
       <c r="G130" s="5"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5073,7 +5064,7 @@
       </c>
       <c r="G131" s="5"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5094,7 +5085,7 @@
       </c>
       <c r="G132" s="5"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5115,7 +5106,7 @@
       </c>
       <c r="G133" s="5"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5136,7 +5127,7 @@
       </c>
       <c r="G134" s="5"/>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5157,7 +5148,7 @@
       </c>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5178,7 +5169,7 @@
       </c>
       <c r="G136" s="5"/>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5199,7 +5190,7 @@
       </c>
       <c r="G137" s="5"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5220,7 +5211,7 @@
       </c>
       <c r="G138" s="5"/>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5241,7 +5232,7 @@
       </c>
       <c r="G139" s="5"/>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5262,7 +5253,7 @@
       </c>
       <c r="G140" s="5"/>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5283,7 +5274,7 @@
       </c>
       <c r="G141" s="5"/>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5304,7 +5295,7 @@
       </c>
       <c r="G142" s="5"/>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5325,7 +5316,7 @@
       </c>
       <c r="G143" s="5"/>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="5">
         <f t="shared" ref="A144:A201" si="9">B144*24</f>
         <v>0</v>
@@ -5346,7 +5337,7 @@
       </c>
       <c r="G144" s="5"/>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5367,7 +5358,7 @@
       </c>
       <c r="G145" s="5"/>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5388,7 +5379,7 @@
       </c>
       <c r="G146" s="5"/>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5409,7 +5400,7 @@
       </c>
       <c r="G147" s="5"/>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5430,7 +5421,7 @@
       </c>
       <c r="G148" s="5"/>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5451,7 +5442,7 @@
       </c>
       <c r="G149" s="5"/>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5472,7 +5463,7 @@
       </c>
       <c r="G150" s="5"/>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5493,7 +5484,7 @@
       </c>
       <c r="G151" s="5"/>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5514,7 +5505,7 @@
       </c>
       <c r="G152" s="5"/>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5535,7 +5526,7 @@
       </c>
       <c r="G153" s="5"/>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5556,7 +5547,7 @@
       </c>
       <c r="G154" s="5"/>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5577,7 +5568,7 @@
       </c>
       <c r="G155" s="5"/>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5598,7 +5589,7 @@
       </c>
       <c r="G156" s="5"/>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5619,7 +5610,7 @@
       </c>
       <c r="G157" s="5"/>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5640,7 +5631,7 @@
       </c>
       <c r="G158" s="5"/>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5661,7 +5652,7 @@
       </c>
       <c r="G159" s="5"/>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5682,7 +5673,7 @@
       </c>
       <c r="G160" s="5"/>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5703,7 +5694,7 @@
       </c>
       <c r="G161" s="5"/>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5724,7 +5715,7 @@
       </c>
       <c r="G162" s="5"/>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5745,7 +5736,7 @@
       </c>
       <c r="G163" s="5"/>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5766,7 +5757,7 @@
       </c>
       <c r="G164" s="5"/>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5787,7 +5778,7 @@
       </c>
       <c r="G165" s="5"/>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5808,7 +5799,7 @@
       </c>
       <c r="G166" s="5"/>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5829,7 +5820,7 @@
       </c>
       <c r="G167" s="5"/>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5850,7 +5841,7 @@
       </c>
       <c r="G168" s="5"/>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5871,7 +5862,7 @@
       </c>
       <c r="G169" s="5"/>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5892,7 +5883,7 @@
       </c>
       <c r="G170" s="5"/>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5913,7 +5904,7 @@
       </c>
       <c r="G171" s="5"/>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5934,7 +5925,7 @@
       </c>
       <c r="G172" s="5"/>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5955,7 +5946,7 @@
       </c>
       <c r="G173" s="5"/>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5976,7 +5967,7 @@
       </c>
       <c r="G174" s="5"/>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5997,7 +5988,7 @@
       </c>
       <c r="G175" s="5"/>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6018,7 +6009,7 @@
       </c>
       <c r="G176" s="5"/>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6039,7 +6030,7 @@
       </c>
       <c r="G177" s="5"/>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6060,7 +6051,7 @@
       </c>
       <c r="G178" s="5"/>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6081,7 +6072,7 @@
       </c>
       <c r="G179" s="5"/>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6102,7 +6093,7 @@
       </c>
       <c r="G180" s="5"/>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6123,7 +6114,7 @@
       </c>
       <c r="G181" s="5"/>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6144,7 +6135,7 @@
       </c>
       <c r="G182" s="5"/>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6165,7 +6156,7 @@
       </c>
       <c r="G183" s="5"/>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6186,7 +6177,7 @@
       </c>
       <c r="G184" s="5"/>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6207,7 +6198,7 @@
       </c>
       <c r="G185" s="5"/>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6228,7 +6219,7 @@
       </c>
       <c r="G186" s="5"/>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6249,7 +6240,7 @@
       </c>
       <c r="G187" s="5"/>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6270,7 +6261,7 @@
       </c>
       <c r="G188" s="5"/>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6291,7 +6282,7 @@
       </c>
       <c r="G189" s="5"/>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6312,7 +6303,7 @@
       </c>
       <c r="G190" s="5"/>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6333,7 +6324,7 @@
       </c>
       <c r="G191" s="5"/>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6354,7 +6345,7 @@
       </c>
       <c r="G192" s="5"/>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6375,7 +6366,7 @@
       </c>
       <c r="G193" s="5"/>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6396,7 +6387,7 @@
       </c>
       <c r="G194" s="5"/>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6417,7 +6408,7 @@
       </c>
       <c r="G195" s="5"/>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6438,7 +6429,7 @@
       </c>
       <c r="G196" s="5"/>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6459,7 +6450,7 @@
       </c>
       <c r="G197" s="5"/>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6480,7 +6471,7 @@
       </c>
       <c r="G198" s="5"/>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6501,7 +6492,7 @@
       </c>
       <c r="G199" s="5"/>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6522,7 +6513,7 @@
       </c>
       <c r="G200" s="5"/>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6536,6 +6527,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -6548,9 +6540,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -6558,7 +6550,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -6566,7 +6558,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>39</v>
       </c>
@@ -6582,7 +6574,7 @@
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>41</v>
       </c>
@@ -6598,7 +6590,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>0.46875</v>
       </c>
@@ -6606,7 +6598,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>0.47638888888888892</v>
       </c>
@@ -6614,7 +6606,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>0.4861111111111111</v>
       </c>
@@ -6622,7 +6614,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>0.48749999999999999</v>
       </c>
@@ -6630,7 +6622,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>0.49305555555555558</v>
       </c>
@@ -6638,7 +6630,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>0.49583333333333335</v>
       </c>
@@ -6646,7 +6638,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>0.50208333333333333</v>
       </c>
@@ -6654,7 +6646,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <v>0.50972222222222219</v>
       </c>
@@ -6662,7 +6654,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <v>0.5229166666666667</v>
       </c>
@@ -6670,7 +6662,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
         <v>0.53611111111111109</v>
       </c>
@@ -6678,7 +6670,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <v>0.53819444444444442</v>
       </c>
@@ -6686,7 +6678,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
         <v>0.54513888888888895</v>
       </c>
@@ -6694,7 +6686,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
         <v>0.54861111111111105</v>
       </c>
@@ -6702,7 +6694,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
         <v>0.5493055555555556</v>
       </c>
@@ -6710,7 +6702,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
         <v>0.56527777777777777</v>
       </c>
@@ -6718,7 +6710,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
         <v>0.57013888888888886</v>
       </c>
@@ -6726,7 +6718,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <v>0.57291666666666663</v>
       </c>
@@ -6734,7 +6726,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
         <v>0.57430555555555551</v>
       </c>
@@ -6742,7 +6734,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="15">
         <v>0.59097222222222223</v>
       </c>
@@ -6750,7 +6742,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="15">
         <v>0.59375</v>
       </c>
@@ -6758,7 +6750,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="15">
         <v>0.59375</v>
       </c>
@@ -6766,7 +6758,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="15">
         <v>0.59513888888888888</v>
       </c>
@@ -6774,7 +6766,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
         <v>0.59722222222222221</v>
       </c>
@@ -6782,7 +6774,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="15">
         <v>0.60277777777777775</v>
       </c>
@@ -6790,7 +6782,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="15">
         <v>0.60416666666666663</v>
       </c>
@@ -6798,7 +6790,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="15">
         <v>0.60625000000000007</v>
       </c>
@@ -6806,7 +6798,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="15">
         <v>0.62291666666666667</v>
       </c>
@@ -6814,7 +6806,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <v>0.63263888888888886</v>
       </c>
@@ -6822,7 +6814,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="15">
         <v>0.6333333333333333</v>
       </c>
@@ -6830,7 +6822,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="15">
         <v>0.63402777777777775</v>
       </c>
@@ -6838,7 +6830,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <v>0.64374999999999993</v>
       </c>
@@ -6846,7 +6838,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="15">
         <v>0.65069444444444446</v>
       </c>
@@ -6854,7 +6846,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="15">
         <v>0.65138888888888891</v>
       </c>
@@ -6862,7 +6854,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="15">
         <v>0.66388888888888886</v>
       </c>
@@ -6870,7 +6862,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <v>0.67083333333333339</v>
       </c>
@@ -6878,7 +6870,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="15">
         <v>0.67638888888888893</v>
       </c>
@@ -6886,7 +6878,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="15">
         <v>0.68611111111111101</v>
       </c>
@@ -6894,7 +6886,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="15">
         <v>0.69305555555555554</v>
       </c>
@@ -6902,7 +6894,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <v>0.69861111111111107</v>
       </c>
@@ -6910,7 +6902,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="15">
         <v>0.70138888888888884</v>
       </c>
@@ -6918,7 +6910,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="15">
         <v>0.70277777777777783</v>
       </c>
@@ -6926,43 +6918,43 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="15"/>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="15"/>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="15"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="15"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="15"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="15"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="15"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="15"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="15"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="15"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="15"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="15"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="15"/>
     </row>
   </sheetData>
@@ -6978,17 +6970,17 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>69</v>
       </c>
@@ -6996,7 +6988,7 @@
         <v>333.72</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.75" customHeight="1">
+    <row r="4" spans="1:3" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
         <v>70</v>
       </c>
@@ -7004,7 +6996,7 @@
         <v>118.08</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>71</v>
       </c>
@@ -7019,6 +7011,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6a0c5501-c863-4286-a1b2-b3df72dde9d2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9f6ff15b-5c0d-4cbb-8f2a-60d7608b85b9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010021525640E197524BB9BF0238C7DE8EF0" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5f90b18cafaa620c655dfdc2a141fe2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6a0c5501-c863-4286-a1b2-b3df72dde9d2" xmlns:ns3="9f6ff15b-5c0d-4cbb-8f2a-60d7608b85b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4839e960e6e9fdb62fa500d4cb5d063" ns2:_="" ns3:_="">
     <xsd:import namespace="6a0c5501-c863-4286-a1b2-b3df72dde9d2"/>
@@ -7259,34 +7271,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6a0c5501-c863-4286-a1b2-b3df72dde9d2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9f6ff15b-5c0d-4cbb-8f2a-60d7608b85b9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC678BDB-627F-44C3-ABDF-B6E4586A7159}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81D6CC55-EAF7-4C55-BA00-5929BF905832}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BEECD1C-D056-4B80-8C51-072827413DB9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BEECD1C-D056-4B80-8C51-072827413DB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6a0c5501-c863-4286-a1b2-b3df72dde9d2"/>
+    <ds:schemaRef ds:uri="9f6ff15b-5c0d-4cbb-8f2a-60d7608b85b9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81D6CC55-EAF7-4C55-BA00-5929BF905832}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC678BDB-627F-44C3-ABDF-B6E4586A7159}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6a0c5501-c863-4286-a1b2-b3df72dde9d2"/>
+    <ds:schemaRef ds:uri="9f6ff15b-5c0d-4cbb-8f2a-60d7608b85b9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>